<commit_message>
Added time for morning chores
</commit_message>
<xml_diff>
--- a/ProjectDoc/!Task Log future SCM.xlsx
+++ b/ProjectDoc/!Task Log future SCM.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="510" yWindow="570" windowWidth="18855" windowHeight="11955"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
   <si>
     <t>Task/Activity</t>
   </si>
@@ -19,7 +22,7 @@
     <t>Doc/Component</t>
   </si>
   <si>
-    <t>What </t>
+    <t>What</t>
   </si>
   <si>
     <t>'Check in'</t>
@@ -208,42 +211,93 @@
   </si>
   <si>
     <t>Docs from google drive to repos directory</t>
+  </si>
+  <si>
+    <t>GPTree.java</t>
+  </si>
+  <si>
+    <t>Checked src into GitHub</t>
+  </si>
+  <si>
+    <t>(commit ID?)</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>from the zip Li sent on Mon 25th</t>
+  </si>
+  <si>
+    <t>Added "0" to operands</t>
+  </si>
+  <si>
+    <t>recalled from team meeting; did not test</t>
+  </si>
+  <si>
+    <t>checked in clean ProjectPlan</t>
+  </si>
+  <si>
+    <t>ProjectPlan.docx</t>
+  </si>
+  <si>
+    <t>from email Oct 25</t>
+  </si>
+  <si>
+    <t>added new prost-project analysis</t>
+  </si>
+  <si>
+    <t>from Justin</t>
+  </si>
+  <si>
+    <t>added assgn 10</t>
+  </si>
+  <si>
+    <t>from Roger</t>
+  </si>
+  <si>
+    <t>SWAssign1-_Sat_13F</t>
+  </si>
+  <si>
+    <t>PCR-1 Requirement Change Action.txt</t>
+  </si>
+  <si>
+    <t>Req Change Analysis</t>
+  </si>
+  <si>
+    <t>Requirement Change to Git</t>
+  </si>
+  <si>
+    <t>Save requirements change request to project</t>
+  </si>
+  <si>
+    <t>Req Change Analysis - training data analysis</t>
+  </si>
+  <si>
+    <t>Req Change Analysis with Training Data.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -253,9 +307,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -318,502 +370,964 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="0" fontId="0" applyNumberFormat="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="165" borderId="1" fontId="0" applyNumberFormat="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="166" borderId="0" fontId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="4" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="31.71"/>
-    <col min="3" customWidth="1" max="3" width="29.86"/>
-    <col min="4" customWidth="1" max="4" width="10.57"/>
-    <col min="5" customWidth="1" max="5" width="18.86"/>
-    <col min="6" customWidth="1" max="6" width="8.71"/>
-    <col min="7" customWidth="1" max="7" width="35.86"/>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="6" r="A2">
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="6" r="B2">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="6" r="C2">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="6" r="D2">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="6" r="E2">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="6" r="F2">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="G2">
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="5" r="A3">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="5" r="B3">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="5" r="C3">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c s="2" r="D3">
+      <c r="D3" s="2">
         <v>41537</v>
       </c>
-      <c t="s" s="7" r="E3">
-        <v>12</v>
-      </c>
-      <c s="7" r="F3">
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7">
         <v>2.5</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="7" r="A4">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="7" r="B4">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="7" r="C4">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c s="1" r="D4">
+      <c r="D4" s="1">
         <v>41562</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="D5">
+      <c r="D5" s="1">
         <v>41562</v>
       </c>
-      <c t="s" r="E5">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" r="A6">
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c s="1" r="D6">
+      <c r="D6" s="1">
         <v>41562</v>
       </c>
-      <c t="s" r="E6">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" r="A7">
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c s="1" r="D7">
+      <c r="D7" s="1">
         <v>41569</v>
       </c>
-      <c t="s" r="E7">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7">
         <v>2.5</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" r="A8">
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c s="1" r="D8">
+      <c r="D8" s="1">
         <v>41565</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8">
         <v>0.75</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" r="A9">
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c s="1" r="D9">
+      <c r="D9" s="1">
         <v>41571</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" r="A10">
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c s="1" r="D10">
+      <c r="D10" s="1">
         <v>41571</v>
       </c>
-      <c t="s" r="E10">
+      <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10">
         <v>2.5</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" r="A11">
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c s="1" r="D11">
+      <c r="D11" s="1">
         <v>41572</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" t="s">
         <v>12</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" r="A12">
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c s="1" r="D12">
+      <c r="D12" s="1">
         <v>41572</v>
       </c>
-      <c t="s" r="E12">
+      <c r="E12" t="s">
         <v>12</v>
       </c>
       <c r="F12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" r="A13">
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c s="1" r="D13">
+      <c r="D13" s="1">
         <v>41572</v>
       </c>
-      <c t="s" r="E13">
+      <c r="E13" t="s">
         <v>12</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
-      <c t="s" r="G13">
+      <c r="G13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" r="A14">
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c s="1" r="D14">
+      <c r="D14" s="1">
         <v>41570</v>
       </c>
-      <c t="s" r="E14">
+      <c r="E14" t="s">
         <v>35</v>
       </c>
       <c r="F14">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" r="A15">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="C15">
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c s="1" r="D15">
+      <c r="D15" s="1">
         <v>41571</v>
       </c>
-      <c t="s" r="E15">
+      <c r="E15" t="s">
         <v>35</v>
       </c>
       <c r="F15">
         <v>1.5</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" r="A16">
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c s="1" r="D16">
+      <c r="D16" s="1">
         <v>41576</v>
       </c>
-      <c t="s" r="E16">
+      <c r="E16" t="s">
         <v>37</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
-      <c t="s" r="G16">
+      <c r="G16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" r="A17">
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c s="1" r="D17">
+      <c r="D17" s="1">
         <v>41580</v>
       </c>
-      <c t="s" r="E17">
+      <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
-      <c t="s" r="G17">
+      <c r="G17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" r="A18">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c t="s" r="C18">
+      <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c s="1" r="D18">
+      <c r="D18" s="1">
         <v>41583</v>
       </c>
-      <c t="s" r="E18">
+      <c r="E18" t="s">
         <v>43</v>
       </c>
       <c r="F18">
         <v>0.7</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" r="A19">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c t="s" r="C19">
+      <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c s="1" r="D19">
+      <c r="D19" s="1">
         <v>41590</v>
       </c>
-      <c t="s" r="E19">
+      <c r="E19" t="s">
         <v>46</v>
       </c>
       <c r="F19">
         <v>1.5</v>
       </c>
-      <c t="s" r="G19">
+      <c r="G19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="4" r="A20">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="4" r="B20">
+      <c r="B20" s="4" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="4" r="C20">
+      <c r="C20" s="4" t="s">
         <v>50</v>
       </c>
-      <c s="3" r="D20">
+      <c r="D20" s="3">
         <v>41571</v>
       </c>
-      <c t="s" s="4" r="E20">
+      <c r="E20" s="4" t="s">
         <v>51</v>
       </c>
-      <c s="4" r="F20"/>
-      <c s="4" r="G20"/>
-    </row>
-    <row r="21">
-      <c t="s" s="4" r="A21">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="4" r="B21">
+      <c r="B21" s="4" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="4" r="C21">
+      <c r="C21" s="4" t="s">
         <v>54</v>
       </c>
-      <c s="3" r="D21">
+      <c r="D21" s="3">
         <v>41571</v>
       </c>
-      <c t="s" s="4" r="E21">
+      <c r="E21" s="4" t="s">
         <v>55</v>
       </c>
-      <c s="4" r="F21"/>
-      <c s="4" r="G21"/>
-    </row>
-    <row r="22">
-      <c t="s" s="4" r="A22">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="4" r="B22">
+      <c r="B22" s="4" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="4" r="C22">
+      <c r="C22" s="4" t="s">
         <v>50</v>
       </c>
-      <c s="3" r="D22">
+      <c r="D22" s="3">
         <v>41572</v>
       </c>
-      <c t="s" s="4" r="E22">
+      <c r="E22" s="4" t="s">
         <v>57</v>
       </c>
-      <c s="4" r="F22"/>
-      <c s="4" r="G22"/>
-    </row>
-    <row r="23">
-      <c t="s" s="4" r="A23">
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
-      <c s="4" r="B23"/>
-      <c s="4" r="C23"/>
-      <c s="3" r="D23">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3">
         <v>41591</v>
       </c>
-      <c t="s" s="4" r="E23">
+      <c r="E23" s="4" t="s">
         <v>57</v>
       </c>
-      <c s="4" r="F23"/>
-      <c s="4" r="G23"/>
-    </row>
-    <row r="24">
-      <c t="s" s="4" r="A24">
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>59</v>
       </c>
-      <c s="4" r="B24"/>
-      <c t="s" s="4" r="C24">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="4" r="D24">
+      <c r="D24" s="4" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="4" r="E24">
+      <c r="E24" s="4" t="s">
         <v>35</v>
       </c>
-      <c s="4" r="F24"/>
-      <c s="4" r="G24"/>
-    </row>
-    <row r="25">
-      <c t="s" r="A25">
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>62</v>
       </c>
-      <c t="s" r="C25">
+      <c r="C25" t="s">
         <v>63</v>
       </c>
-      <c s="1" r="D25">
+      <c r="D25" s="1">
         <v>41591</v>
       </c>
-      <c t="s" r="E25">
+      <c r="E25" t="s">
         <v>12</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
-      <c t="s" r="G25">
+      <c r="G25" t="s">
         <v>64</v>
       </c>
     </row>
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>0.1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30">
+        <v>0.1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>0.75</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added SCM log data
</commit_message>
<xml_diff>
--- a/ProjectDoc/!Task Log future SCM.xlsx
+++ b/ProjectDoc/!Task Log future SCM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roger Peterson\Documents\GitHub\GPGenie\ProjectDoc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="510" yWindow="570" windowWidth="18855" windowHeight="11955"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="114">
   <si>
     <t>Task/Activity</t>
   </si>
@@ -274,6 +279,90 @@
   </si>
   <si>
     <t>Req Change Analysis with Training Data.xlsx</t>
+  </si>
+  <si>
+    <t>Added test case reference</t>
+  </si>
+  <si>
+    <t>CID e5f342d</t>
+  </si>
+  <si>
+    <t>Added cell # and assn 10</t>
+  </si>
+  <si>
+    <t>CID 5d2f5d9</t>
+  </si>
+  <si>
+    <t>Phone # and doc</t>
+  </si>
+  <si>
+    <t>Updated assn 10</t>
+  </si>
+  <si>
+    <t>CID 8c3aed0</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>Tracebility matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added test case design </t>
+  </si>
+  <si>
+    <t>CID 5s70281</t>
+  </si>
+  <si>
+    <t>Revised test case design</t>
+  </si>
+  <si>
+    <t>CID d7aa179</t>
+  </si>
+  <si>
+    <t>Document revision</t>
+  </si>
+  <si>
+    <t>Test case design.xls</t>
+  </si>
+  <si>
+    <t>Proposed change mangement diagram</t>
+  </si>
+  <si>
+    <t>CID 8d4e101</t>
+  </si>
+  <si>
+    <t>Change mangement.ppt</t>
+  </si>
+  <si>
+    <t>Proposed assignment 10 .ppt</t>
+  </si>
+  <si>
+    <t>CID 317401e</t>
+  </si>
+  <si>
+    <t>Assn 10 .ppt</t>
+  </si>
+  <si>
+    <t>Updated assn 10 and traceability matrix</t>
+  </si>
+  <si>
+    <t>Revised existing docs</t>
+  </si>
+  <si>
+    <t>CID 237a8c4</t>
+  </si>
+  <si>
+    <t>In care of Susan</t>
+  </si>
+  <si>
+    <t>Created RSC spreadsheet for GP Genie</t>
+  </si>
+  <si>
+    <t>CID 870b9d0</t>
+  </si>
+  <si>
+    <t>SW measurement tool</t>
   </si>
 </sst>
 </file>
@@ -413,6 +502,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -460,7 +552,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,7 +587,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -704,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1310,7 +1402,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -1325,6 +1417,189 @@
       </c>
       <c r="F33">
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="9">
+        <v>41610</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="9">
+        <v>41611</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="9">
+        <v>41611</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="9">
+        <v>41613</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="9">
+        <v>41615</v>
+      </c>
+      <c r="E39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="9">
+        <v>41615</v>
+      </c>
+      <c r="E40" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="9">
+        <v>41615</v>
+      </c>
+      <c r="E41" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="9">
+        <v>41616</v>
+      </c>
+      <c r="E42" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated my time (in progress)
</commit_message>
<xml_diff>
--- a/ProjectDoc/!Task Log future SCM.xlsx
+++ b/ProjectDoc/!Task Log future SCM.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roger Peterson\Documents\GitHub\GPGenie\ProjectDoc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="510" yWindow="570" windowWidth="18855" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="143">
   <si>
     <t>Task/Activity</t>
   </si>
@@ -378,6 +373,78 @@
   </si>
   <si>
     <t>CID 2917998</t>
+  </si>
+  <si>
+    <t>code merge correction</t>
+  </si>
+  <si>
+    <t>CID d61fbe1</t>
+  </si>
+  <si>
+    <t>Code check-in collision</t>
+  </si>
+  <si>
+    <t>final design doc &amp; add to report</t>
+  </si>
+  <si>
+    <t>test run: functional testing to analyse bad fitness values</t>
+  </si>
+  <si>
+    <t>FuncitnalTestRunsFitness.xlsx</t>
+  </si>
+  <si>
+    <t>CID 37c8bc1</t>
+  </si>
+  <si>
+    <t>Final Class Diagram visio, report</t>
+  </si>
+  <si>
+    <t>CID 95d0b09</t>
+  </si>
+  <si>
+    <t>mutation.java</t>
+  </si>
+  <si>
+    <t>check in mutation update from Li</t>
+  </si>
+  <si>
+    <t>analysis and solving readable tree format</t>
+  </si>
+  <si>
+    <t>CID 8c5b78b</t>
+  </si>
+  <si>
+    <t>Java code;</t>
+  </si>
+  <si>
+    <t>analysis of usable print test results in fitness evaluator spreadsheets</t>
+  </si>
+  <si>
+    <t>analysis and review of the fitness output defect</t>
+  </si>
+  <si>
+    <t>Li &amp; Susan</t>
+  </si>
+  <si>
+    <t>Ongoing - Li and Susan together</t>
+  </si>
+  <si>
+    <t>CID b0f3d7f</t>
+  </si>
+  <si>
+    <t>CID 72e7c66</t>
+  </si>
+  <si>
+    <t>CodeTestingEarlyAnalysis.xlsx</t>
+  </si>
+  <si>
+    <t>functional test runs and captures for test plan scripts</t>
+  </si>
+  <si>
+    <t>CID 4ea9f4f</t>
+  </si>
+  <si>
+    <t>FunctionalTestRunsFitness.xlsx</t>
   </si>
 </sst>
 </file>
@@ -398,12 +465,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -576,7 +645,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,7 +680,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -820,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1666,6 +1735,166 @@
         <v>0.75</v>
       </c>
     </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="9">
+        <v>41620</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" s="9">
+        <v>41620</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D54" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added time back two weeks
</commit_message>
<xml_diff>
--- a/ProjectDoc/!Task Log future SCM.xlsx
+++ b/ProjectDoc/!Task Log future SCM.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$G$60</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="165">
   <si>
     <t>Task/Activity</t>
   </si>
@@ -445,6 +448,72 @@
   </si>
   <si>
     <t>FunctionalTestRunsFitness.xlsx</t>
+  </si>
+  <si>
+    <t>Team Meeting</t>
+  </si>
+  <si>
+    <t>U, L, R, F, J, S</t>
+  </si>
+  <si>
+    <t>Updated report, slides, code</t>
+  </si>
+  <si>
+    <t>Test Captures</t>
+  </si>
+  <si>
+    <t>CID 82fd6a9</t>
+  </si>
+  <si>
+    <t>Code testing for fitness; test results updates</t>
+  </si>
+  <si>
+    <t>Slide development</t>
+  </si>
+  <si>
+    <t>emailed</t>
+  </si>
+  <si>
+    <t>final preso to Ujin</t>
+  </si>
+  <si>
+    <t>User testing for valid, invalid data entry</t>
+  </si>
+  <si>
+    <t>CID b98994c</t>
+  </si>
+  <si>
+    <t>Working Meeting</t>
+  </si>
+  <si>
+    <t>Code, Test, PPT, Report content</t>
+  </si>
+  <si>
+    <t>R, U, S, F, L</t>
+  </si>
+  <si>
+    <t>Working online meeting - code work</t>
+  </si>
+  <si>
+    <t>Review of code, walkthroughs for code reviews</t>
+  </si>
+  <si>
+    <t>L, S</t>
+  </si>
+  <si>
+    <t>Early code familiarity and review</t>
+  </si>
+  <si>
+    <t>Working Meeting on site</t>
+  </si>
+  <si>
+    <t>Review of code, report,project needs</t>
+  </si>
+  <si>
+    <t>U, L, S, R, F, J</t>
+  </si>
+  <si>
+    <t>Working through each module, early output investigation</t>
   </si>
 </sst>
 </file>
@@ -889,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1614,33 +1683,30 @@
     </row>
     <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
       <c r="D39" s="9">
-        <v>41615</v>
+        <v>41614</v>
       </c>
       <c r="E39" t="s">
-        <v>57</v>
+        <v>156</v>
       </c>
       <c r="F39">
-        <v>0.75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D40" s="9">
         <v>41615</v>
@@ -1649,18 +1715,18 @@
         <v>57</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D41" s="9">
         <v>41615</v>
@@ -1669,24 +1735,21 @@
         <v>57</v>
       </c>
       <c r="F41">
-        <v>2</v>
-      </c>
-      <c r="G41" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D42" s="9">
-        <v>41616</v>
+        <v>41615</v>
       </c>
       <c r="E42" t="s">
         <v>57</v>
@@ -1694,44 +1757,118 @@
       <c r="F42">
         <v>2</v>
       </c>
+      <c r="G42" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="9">
+        <v>41615</v>
+      </c>
+      <c r="E43" t="s">
+        <v>159</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="9">
+        <v>41616</v>
+      </c>
+      <c r="E44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="9">
+        <v>41617</v>
+      </c>
+      <c r="E45" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="9">
+        <v>41617</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>114</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B47" t="s">
         <v>115</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C47" t="s">
         <v>116</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D47" s="9">
         <v>41620</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E47" t="s">
         <v>57</v>
       </c>
-      <c r="F43">
+      <c r="F47">
         <v>0.75</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+    <row r="48" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B48" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D48" s="9">
         <v>41620</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E48" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F44">
+      <c r="F48">
         <v>0.75</v>
       </c>
     </row>
@@ -1893,6 +2030,86 @@
       </c>
       <c r="F56">
         <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E57" t="s">
+        <v>144</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="9">
+        <v>41622</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="9">
+        <v>41622</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" s="9">
+        <v>41622</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated and little changes
</commit_message>
<xml_diff>
--- a/ProjectDoc/!Task Log future SCM.xlsx
+++ b/ProjectDoc/!Task Log future SCM.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="570" windowWidth="18855" windowHeight="11955"/>
+    <workbookView xWindow="520" yWindow="580" windowWidth="22820" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$G$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$G$61</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="171">
   <si>
     <t>Task/Activity</t>
   </si>
@@ -514,6 +519,24 @@
   </si>
   <si>
     <t>Working through each module, early output investigation</t>
+  </si>
+  <si>
+    <t>Project Final Report</t>
+  </si>
+  <si>
+    <t>Project PPT</t>
+  </si>
+  <si>
+    <t>Project Plan - Schedule and Roles</t>
+  </si>
+  <si>
+    <t>Project Plan - Work Plan</t>
+  </si>
+  <si>
+    <t>Ujin</t>
+  </si>
+  <si>
+    <t>Final Report.doc</t>
   </si>
 </sst>
 </file>
@@ -523,7 +546,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -548,6 +571,18 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -582,7 +617,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -591,10 +626,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,7 +638,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,14 +646,16 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -655,7 +692,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,23 +997,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -982,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="12.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +1044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +1064,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1065,7 +1104,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1082,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1102,7 +1141,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1116,29 +1155,29 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="12.75" customHeight="1">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1">
-        <v>41571</v>
+        <v>168</v>
+      </c>
+      <c r="D9" s="9">
+        <v>41570</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>169</v>
       </c>
       <c r="F9">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1">
         <v>41571</v>
@@ -1147,32 +1186,32 @@
         <v>12</v>
       </c>
       <c r="F10">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1">
+        <v>41571</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="1">
-        <v>41572</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
       </c>
       <c r="D12" s="1">
         <v>41572</v>
@@ -1181,15 +1220,15 @@
         <v>12</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1">
         <v>41572</v>
@@ -1198,30 +1237,30 @@
         <v>12</v>
       </c>
       <c r="F13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1">
+        <v>41572</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
         <v>2</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="1">
-        <v>41570</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1229,151 +1268,153 @@
         <v>34</v>
       </c>
       <c r="D15" s="1">
-        <v>41571</v>
+        <v>41570</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
       <c r="F15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1">
+        <v>41571</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
         <v>41576</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>37</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>1</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
         <v>41580</v>
       </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17">
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
         <v>2</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
         <v>41583</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>43</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
         <v>41590</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>1.5</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D20" s="3">
-        <v>41571</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D21" s="3">
         <v>41571</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D22" s="3">
-        <v>41572</v>
+        <v>41571</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="D23" s="3">
-        <v>41591</v>
+        <v>41572</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>57</v>
@@ -1381,75 +1422,67 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>61</v>
+      <c r="C24" s="4"/>
+      <c r="D24" s="3">
+        <v>41591</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A26" t="s">
         <v>62</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>41591</v>
       </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25">
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26">
         <v>1</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A27" t="s">
         <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="9">
-        <v>41610</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26">
-        <v>0.5</v>
-      </c>
-      <c r="G26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D27" s="9">
         <v>41610</v>
@@ -1458,21 +1491,21 @@
         <v>12</v>
       </c>
       <c r="F27">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="12.75" customHeight="1">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
         <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D28" s="9">
         <v>41610</v>
@@ -1484,16 +1517,19 @@
         <v>0.1</v>
       </c>
       <c r="G28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="12.75" customHeight="1">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
         <v>67</v>
       </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
       <c r="D29" s="9">
         <v>41610</v>
       </c>
@@ -1504,19 +1540,16 @@
         <v>0.1</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="12.75" customHeight="1">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
         <v>67</v>
       </c>
-      <c r="C30" t="s">
-        <v>79</v>
-      </c>
       <c r="D30" s="9">
         <v>41610</v>
       </c>
@@ -1527,15 +1560,18 @@
         <v>0.1</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="12.75" customHeight="1">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="9">
         <v>41610</v>
@@ -1544,15 +1580,18 @@
         <v>12</v>
       </c>
       <c r="F31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D32" s="9">
         <v>41610</v>
@@ -1561,15 +1600,15 @@
         <v>12</v>
       </c>
       <c r="F32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D33" s="9">
         <v>41610</v>
@@ -1578,38 +1617,35 @@
         <v>12</v>
       </c>
       <c r="F33">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D34" s="9">
         <v>41610</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="F34">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="12.75" customHeight="1">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D35" s="9">
         <v>41610</v>
@@ -1618,38 +1654,38 @@
         <v>57</v>
       </c>
       <c r="F35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D36" s="9">
-        <v>41611</v>
+        <v>41610</v>
       </c>
       <c r="E36" t="s">
         <v>57</v>
       </c>
       <c r="F36">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D37" s="9">
         <v>41611</v>
@@ -1658,75 +1694,75 @@
         <v>57</v>
       </c>
       <c r="F37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="12.75" customHeight="1">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D38" s="9">
-        <v>41613</v>
+        <v>41611</v>
       </c>
       <c r="E38" t="s">
         <v>57</v>
       </c>
       <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="9">
+        <v>41613</v>
+      </c>
+      <c r="E39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39">
         <v>0.75</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A40" t="s">
         <v>154</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>155</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D40" s="9">
         <v>41614</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>156</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A41" t="s">
         <v>101</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>102</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>103</v>
-      </c>
-      <c r="D40" s="9">
-        <v>41615</v>
-      </c>
-      <c r="E40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" t="s">
-        <v>106</v>
       </c>
       <c r="D41" s="9">
         <v>41615</v>
@@ -1735,18 +1771,18 @@
         <v>57</v>
       </c>
       <c r="F41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D42" s="9">
         <v>41615</v>
@@ -1755,212 +1791,212 @@
         <v>57</v>
       </c>
       <c r="F42">
-        <v>2</v>
-      </c>
-      <c r="G42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>107</v>
+      </c>
+      <c r="B43" t="s">
+        <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="D43" s="9">
         <v>41615</v>
       </c>
       <c r="E43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="9">
+        <v>41615</v>
+      </c>
+      <c r="E44" t="s">
         <v>159</v>
       </c>
-      <c r="F43">
+      <c r="F44">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A45" t="s">
         <v>111</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>112</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D45" s="9">
         <v>41616</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>57</v>
-      </c>
-      <c r="F44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>161</v>
-      </c>
-      <c r="C45" t="s">
-        <v>162</v>
-      </c>
-      <c r="D45" s="9">
-        <v>41617</v>
-      </c>
-      <c r="E45" t="s">
-        <v>163</v>
       </c>
       <c r="F45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C46" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D46" s="9">
         <v>41617</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>163</v>
       </c>
       <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="27" customHeight="1">
+      <c r="A47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="9">
+        <v>41617</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A48" t="s">
         <v>114</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>115</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>116</v>
-      </c>
-      <c r="D47" s="9">
-        <v>41620</v>
-      </c>
-      <c r="E47" t="s">
-        <v>57</v>
-      </c>
-      <c r="F47">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="D48" s="9">
         <v>41620</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" t="s">
         <v>57</v>
       </c>
       <c r="F48">
         <v>0.75</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="12.75" customHeight="1">
       <c r="A49" s="10" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="D49" s="9">
         <v>41620</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="F49">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="12">
+      <c r="A50" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="9">
+        <v>41620</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
+    <row r="51" spans="1:6" ht="12">
+      <c r="A51" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B51" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C51" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D51" s="9">
         <v>41621</v>
       </c>
-      <c r="E50" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50">
+      <c r="E51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
+    <row r="52" spans="1:6" ht="24">
+      <c r="A52" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C52" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D52" s="9">
         <v>41620</v>
       </c>
-      <c r="E51" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51">
+      <c r="E52" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
+    <row r="53" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A53" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B53" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C53" s="10" t="s">
         <v>128</v>
-      </c>
-      <c r="D52" s="9">
-        <v>41621</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="D53" s="9">
         <v>41621</v>
@@ -1969,18 +2005,18 @@
         <v>12</v>
       </c>
       <c r="F53">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="12.75" customHeight="1">
       <c r="A54" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D54" s="9">
         <v>41621</v>
@@ -1989,18 +2025,18 @@
         <v>12</v>
       </c>
       <c r="F54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="12.75" customHeight="1">
       <c r="A55" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D55" s="9">
         <v>41621</v>
@@ -2012,75 +2048,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="12.75" customHeight="1">
       <c r="A56" s="10" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D56" s="9">
         <v>41621</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>143</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="57" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A57" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C57" t="s">
-        <v>145</v>
+      <c r="C57" s="10" t="s">
+        <v>136</v>
       </c>
       <c r="D57" s="9">
         <v>41621</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A58" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E58" t="s">
         <v>144</v>
       </c>
-      <c r="F57">
+      <c r="F58">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A59" t="s">
         <v>149</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>150</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>151</v>
-      </c>
-      <c r="D58" s="9">
-        <v>41622</v>
-      </c>
-      <c r="E58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>148</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C59" t="s">
-        <v>146</v>
       </c>
       <c r="D59" s="9">
         <v>41622</v>
@@ -2089,15 +2125,15 @@
         <v>12</v>
       </c>
       <c r="F59">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>152</v>
-      </c>
-      <c r="B60" t="s">
-        <v>153</v>
+        <v>148</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="C60" t="s">
         <v>146</v>
@@ -2112,7 +2148,73 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="61" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A61" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="9">
+        <v>41622</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A62" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="9">
+        <v>41621</v>
+      </c>
+      <c r="E62" t="s">
+        <v>169</v>
+      </c>
+      <c r="F62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A63" t="s">
+        <v>166</v>
+      </c>
+      <c r="B63" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="9">
+        <v>41622</v>
+      </c>
+      <c r="E63" t="s">
+        <v>169</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>